<commit_message>
Non-final arrays analyzed completely.
</commit_message>
<xml_diff>
--- a/analyzer/results/arrays/nonfinals.xlsx
+++ b/analyzer/results/arrays/nonfinals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\arrays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C980AD0D-CC88-4417-A65B-3E82BCEFB3C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E41608C-0738-4872-B1A4-EF13B2CD067A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>Owner</t>
   </si>
@@ -140,6 +140,27 @@
   </si>
   <si>
     <t>bnExpModThreshTable</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Immutable</t>
+  </si>
+  <si>
+    <t>Effectively immutable</t>
+  </si>
+  <si>
+    <t>Never modified</t>
+  </si>
+  <si>
+    <t>Internal use only</t>
+  </si>
+  <si>
+    <t>after initalization</t>
   </si>
 </sst>
 </file>
@@ -457,15 +478,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C21"/>
+      <selection activeCell="D1" sqref="D1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +503,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -486,8 +520,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -497,8 +537,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -508,8 +554,14 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -519,8 +571,14 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -530,8 +588,14 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -541,8 +605,14 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -552,8 +622,14 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -563,8 +639,14 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -574,8 +656,14 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -585,8 +673,14 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -596,8 +690,14 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -607,8 +707,14 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -618,8 +724,14 @@
       <c r="C14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -629,8 +741,14 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -640,8 +758,14 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -651,8 +775,14 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -662,8 +792,14 @@
       <c r="C18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -673,8 +809,14 @@
       <c r="C19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -684,8 +826,14 @@
       <c r="C20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -695,23 +843,48 @@
       <c r="C21" t="s">
         <v>5</v>
       </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE548E92-C7F7-4070-A1AD-8051A0F10612}">
+          <x14:formula1>
+            <xm:f>reason!$A$1:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:E21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6280A4A-27F6-4C4B-8936-FDAD11B34CE1}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -721,8 +894,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -732,9 +911,27 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AE99EE0-63A5-4B6C-A7D5-FCC76FE63772}">
+          <x14:formula1>
+            <xm:f>reason!$A$1:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:E2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -764,12 +961,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF704508-B361-463F-BEAC-DC1BC845185E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>